<commit_message>
write results to excel
</commit_message>
<xml_diff>
--- a/BubbleSheet/answers.xlsx
+++ b/BubbleSheet/answers.xlsx
@@ -1,35 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed sabry\Downloads\IP project\Image-Processing\BubbleSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Material\3rd CMP\First term\Image processing\Project\Image-processing\BubbleSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7221C368-D1FD-4528-A30A-6B122451FBE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018290E1-0E54-4124-A675-968B91305CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="bubble sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Code</t>
   </si>
   <si>
+    <t>Name</t>
+  </si>
+  <si>
     <t>Q1</t>
   </si>
   <si>
@@ -42,85 +40,76 @@
     <t>Q4</t>
   </si>
   <si>
+    <t>Q6</t>
+  </si>
+  <si>
+    <t>Q7</t>
+  </si>
+  <si>
+    <t>Q8</t>
+  </si>
+  <si>
+    <t>Q9</t>
+  </si>
+  <si>
+    <t>Q10</t>
+  </si>
+  <si>
+    <t>Q11</t>
+  </si>
+  <si>
+    <t>Q12</t>
+  </si>
+  <si>
+    <t>Q13</t>
+  </si>
+  <si>
+    <t>Q14</t>
+  </si>
+  <si>
+    <t>Q15</t>
+  </si>
+  <si>
+    <t>Q16</t>
+  </si>
+  <si>
+    <t>Q17</t>
+  </si>
+  <si>
+    <t>Q18</t>
+  </si>
+  <si>
+    <t>Q19</t>
+  </si>
+  <si>
+    <t>Q20</t>
+  </si>
+  <si>
+    <t>Q21</t>
+  </si>
+  <si>
+    <t>Q22</t>
+  </si>
+  <si>
+    <t>Q23</t>
+  </si>
+  <si>
+    <t>Q24</t>
+  </si>
+  <si>
+    <t>Q25</t>
+  </si>
+  <si>
+    <t>Q26</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
     <t>Q5</t>
-  </si>
-  <si>
-    <t>Q6</t>
-  </si>
-  <si>
-    <t>Q8</t>
-  </si>
-  <si>
-    <t>Q9</t>
-  </si>
-  <si>
-    <t>Q7</t>
-  </si>
-  <si>
-    <t>Q10</t>
-  </si>
-  <si>
-    <t>Q11</t>
-  </si>
-  <si>
-    <t>Q12</t>
-  </si>
-  <si>
-    <t>Q13</t>
-  </si>
-  <si>
-    <t>Q14</t>
-  </si>
-  <si>
-    <t>Q15</t>
-  </si>
-  <si>
-    <t>Q16</t>
-  </si>
-  <si>
-    <t>Q17</t>
-  </si>
-  <si>
-    <t>Q18</t>
-  </si>
-  <si>
-    <t>Q19</t>
-  </si>
-  <si>
-    <t>Q20</t>
-  </si>
-  <si>
-    <t>Q21</t>
-  </si>
-  <si>
-    <t>Q22</t>
-  </si>
-  <si>
-    <t>Q23</t>
-  </si>
-  <si>
-    <t>Q24</t>
-  </si>
-  <si>
-    <t>Q25</t>
-  </si>
-  <si>
-    <t>Q26</t>
-  </si>
-  <si>
-    <t>Q27</t>
-  </si>
-  <si>
-    <t>Q28</t>
-  </si>
-  <si>
-    <t>Q29</t>
-  </si>
-  <si>
-    <t>Q30</t>
-  </si>
-  <si>
-    <t>Student Name</t>
   </si>
 </sst>
 </file>
@@ -221,7 +210,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -256,7 +245,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -438,51 +427,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF1"/>
+  <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="21.88671875" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
       </c>
       <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
         <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
       </c>
       <c r="L1" t="s">
         <v>10</v>
@@ -535,21 +520,352 @@
       <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" t="s">
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="B2" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>30</v>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2" t="b">
+        <v>1</v>
+      </c>
+      <c r="P2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R2" t="b">
+        <v>1</v>
+      </c>
+      <c r="S2" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2" t="b">
+        <v>1</v>
+      </c>
+      <c r="U2" t="b">
+        <v>1</v>
+      </c>
+      <c r="V2" t="b">
+        <v>1</v>
+      </c>
+      <c r="W2" t="b">
+        <v>1</v>
+      </c>
+      <c r="X2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" t="b">
+        <v>1</v>
+      </c>
+      <c r="N3" t="b">
+        <v>1</v>
+      </c>
+      <c r="O3" t="b">
+        <v>1</v>
+      </c>
+      <c r="P3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S3" t="b">
+        <v>1</v>
+      </c>
+      <c r="T3" t="b">
+        <v>1</v>
+      </c>
+      <c r="U3" t="b">
+        <v>1</v>
+      </c>
+      <c r="V3" t="b">
+        <v>1</v>
+      </c>
+      <c r="W3" t="b">
+        <v>1</v>
+      </c>
+      <c r="X3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" t="b">
+        <v>1</v>
+      </c>
+      <c r="N4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O4" t="b">
+        <v>1</v>
+      </c>
+      <c r="P4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="b">
+        <v>1</v>
+      </c>
+      <c r="R4" t="b">
+        <v>1</v>
+      </c>
+      <c r="S4" t="b">
+        <v>1</v>
+      </c>
+      <c r="T4" t="b">
+        <v>1</v>
+      </c>
+      <c r="U4" t="b">
+        <v>1</v>
+      </c>
+      <c r="V4" t="b">
+        <v>1</v>
+      </c>
+      <c r="W4" t="b">
+        <v>1</v>
+      </c>
+      <c r="X4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="Z5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fit with more NEW test cases
</commit_message>
<xml_diff>
--- a/BubbleSheet/answers.xlsx
+++ b/BubbleSheet/answers.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:AU89"/>
+  <dimension ref="A2:AU132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7461,8 +7461,6 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="inlineStr"/>
-      <c r="B89" t="inlineStr"/>
       <c r="C89" t="n">
         <v>1</v>
       </c>
@@ -7596,6 +7594,3000 @@
         <v>0</v>
       </c>
       <c r="AU89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>0</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0</v>
+      </c>
+      <c r="F90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J90" t="n">
+        <v>0</v>
+      </c>
+      <c r="K90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N90" t="n">
+        <v>0</v>
+      </c>
+      <c r="O90" t="n">
+        <v>0</v>
+      </c>
+      <c r="P90" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q90" t="n">
+        <v>0</v>
+      </c>
+      <c r="R90" t="n">
+        <v>0</v>
+      </c>
+      <c r="S90" t="n">
+        <v>0</v>
+      </c>
+      <c r="T90" t="n">
+        <v>0</v>
+      </c>
+      <c r="U90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>0</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0</v>
+      </c>
+      <c r="F91" t="n">
+        <v>0</v>
+      </c>
+      <c r="G91" t="n">
+        <v>0</v>
+      </c>
+      <c r="H91" t="n">
+        <v>0</v>
+      </c>
+      <c r="I91" t="n">
+        <v>0</v>
+      </c>
+      <c r="J91" t="n">
+        <v>0</v>
+      </c>
+      <c r="K91" t="n">
+        <v>0</v>
+      </c>
+      <c r="L91" t="n">
+        <v>0</v>
+      </c>
+      <c r="M91" t="n">
+        <v>0</v>
+      </c>
+      <c r="N91" t="n">
+        <v>0</v>
+      </c>
+      <c r="O91" t="n">
+        <v>0</v>
+      </c>
+      <c r="P91" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q91" t="n">
+        <v>0</v>
+      </c>
+      <c r="R91" t="n">
+        <v>0</v>
+      </c>
+      <c r="S91" t="n">
+        <v>0</v>
+      </c>
+      <c r="T91" t="n">
+        <v>0</v>
+      </c>
+      <c r="U91" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>0</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0</v>
+      </c>
+      <c r="F92" t="n">
+        <v>0</v>
+      </c>
+      <c r="G92" t="n">
+        <v>0</v>
+      </c>
+      <c r="H92" t="n">
+        <v>0</v>
+      </c>
+      <c r="I92" t="n">
+        <v>0</v>
+      </c>
+      <c r="J92" t="n">
+        <v>0</v>
+      </c>
+      <c r="K92" t="n">
+        <v>0</v>
+      </c>
+      <c r="L92" t="n">
+        <v>0</v>
+      </c>
+      <c r="M92" t="n">
+        <v>0</v>
+      </c>
+      <c r="N92" t="n">
+        <v>0</v>
+      </c>
+      <c r="O92" t="n">
+        <v>0</v>
+      </c>
+      <c r="P92" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q92" t="n">
+        <v>0</v>
+      </c>
+      <c r="R92" t="n">
+        <v>0</v>
+      </c>
+      <c r="S92" t="n">
+        <v>0</v>
+      </c>
+      <c r="T92" t="n">
+        <v>0</v>
+      </c>
+      <c r="U92" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>0</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0</v>
+      </c>
+      <c r="F93" t="n">
+        <v>0</v>
+      </c>
+      <c r="G93" t="n">
+        <v>0</v>
+      </c>
+      <c r="H93" t="n">
+        <v>0</v>
+      </c>
+      <c r="I93" t="n">
+        <v>0</v>
+      </c>
+      <c r="J93" t="n">
+        <v>0</v>
+      </c>
+      <c r="K93" t="n">
+        <v>0</v>
+      </c>
+      <c r="L93" t="n">
+        <v>0</v>
+      </c>
+      <c r="M93" t="n">
+        <v>0</v>
+      </c>
+      <c r="N93" t="n">
+        <v>0</v>
+      </c>
+      <c r="O93" t="n">
+        <v>0</v>
+      </c>
+      <c r="P93" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q93" t="n">
+        <v>0</v>
+      </c>
+      <c r="R93" t="n">
+        <v>0</v>
+      </c>
+      <c r="S93" t="n">
+        <v>0</v>
+      </c>
+      <c r="T93" t="n">
+        <v>0</v>
+      </c>
+      <c r="U93" t="n">
+        <v>0</v>
+      </c>
+      <c r="V93" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>0</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0</v>
+      </c>
+      <c r="F94" t="n">
+        <v>0</v>
+      </c>
+      <c r="G94" t="n">
+        <v>0</v>
+      </c>
+      <c r="H94" t="n">
+        <v>0</v>
+      </c>
+      <c r="I94" t="n">
+        <v>0</v>
+      </c>
+      <c r="J94" t="n">
+        <v>0</v>
+      </c>
+      <c r="K94" t="n">
+        <v>0</v>
+      </c>
+      <c r="L94" t="n">
+        <v>0</v>
+      </c>
+      <c r="M94" t="n">
+        <v>0</v>
+      </c>
+      <c r="N94" t="n">
+        <v>0</v>
+      </c>
+      <c r="O94" t="n">
+        <v>0</v>
+      </c>
+      <c r="P94" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q94" t="n">
+        <v>0</v>
+      </c>
+      <c r="R94" t="n">
+        <v>0</v>
+      </c>
+      <c r="S94" t="n">
+        <v>0</v>
+      </c>
+      <c r="T94" t="n">
+        <v>0</v>
+      </c>
+      <c r="U94" t="n">
+        <v>0</v>
+      </c>
+      <c r="V94" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>0</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0</v>
+      </c>
+      <c r="F95" t="n">
+        <v>0</v>
+      </c>
+      <c r="G95" t="n">
+        <v>0</v>
+      </c>
+      <c r="H95" t="n">
+        <v>0</v>
+      </c>
+      <c r="I95" t="n">
+        <v>0</v>
+      </c>
+      <c r="J95" t="n">
+        <v>0</v>
+      </c>
+      <c r="K95" t="n">
+        <v>0</v>
+      </c>
+      <c r="L95" t="n">
+        <v>0</v>
+      </c>
+      <c r="M95" t="n">
+        <v>0</v>
+      </c>
+      <c r="N95" t="n">
+        <v>0</v>
+      </c>
+      <c r="O95" t="n">
+        <v>0</v>
+      </c>
+      <c r="P95" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q95" t="n">
+        <v>0</v>
+      </c>
+      <c r="R95" t="n">
+        <v>0</v>
+      </c>
+      <c r="S95" t="n">
+        <v>0</v>
+      </c>
+      <c r="T95" t="n">
+        <v>0</v>
+      </c>
+      <c r="U95" t="n">
+        <v>0</v>
+      </c>
+      <c r="V95" t="n">
+        <v>0</v>
+      </c>
+      <c r="W95" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>0</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0</v>
+      </c>
+      <c r="E96" t="n">
+        <v>0</v>
+      </c>
+      <c r="F96" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>0</v>
+      </c>
+      <c r="D97" t="n">
+        <v>0</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0</v>
+      </c>
+      <c r="F97" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>0</v>
+      </c>
+      <c r="D98" t="n">
+        <v>0</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0</v>
+      </c>
+      <c r="F98" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>1</v>
+      </c>
+      <c r="D99" t="n">
+        <v>0</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0</v>
+      </c>
+      <c r="F99" t="n">
+        <v>0</v>
+      </c>
+      <c r="G99" t="n">
+        <v>1</v>
+      </c>
+      <c r="H99" t="n">
+        <v>0</v>
+      </c>
+      <c r="I99" t="n">
+        <v>0</v>
+      </c>
+      <c r="J99" t="n">
+        <v>0</v>
+      </c>
+      <c r="K99" t="n">
+        <v>0</v>
+      </c>
+      <c r="L99" t="n">
+        <v>0</v>
+      </c>
+      <c r="M99" t="n">
+        <v>0</v>
+      </c>
+      <c r="N99" t="n">
+        <v>0</v>
+      </c>
+      <c r="O99" t="n">
+        <v>0</v>
+      </c>
+      <c r="P99" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q99" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>1</v>
+      </c>
+      <c r="D100" t="n">
+        <v>0</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0</v>
+      </c>
+      <c r="F100" t="n">
+        <v>0</v>
+      </c>
+      <c r="G100" t="n">
+        <v>1</v>
+      </c>
+      <c r="H100" t="n">
+        <v>0</v>
+      </c>
+      <c r="I100" t="n">
+        <v>0</v>
+      </c>
+      <c r="J100" t="n">
+        <v>0</v>
+      </c>
+      <c r="K100" t="n">
+        <v>0</v>
+      </c>
+      <c r="L100" t="n">
+        <v>1</v>
+      </c>
+      <c r="M100" t="n">
+        <v>0</v>
+      </c>
+      <c r="N100" t="n">
+        <v>0</v>
+      </c>
+      <c r="O100" t="n">
+        <v>0</v>
+      </c>
+      <c r="P100" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q100" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>1</v>
+      </c>
+      <c r="D101" t="n">
+        <v>0</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0</v>
+      </c>
+      <c r="F101" t="n">
+        <v>0</v>
+      </c>
+      <c r="G101" t="n">
+        <v>1</v>
+      </c>
+      <c r="H101" t="n">
+        <v>0</v>
+      </c>
+      <c r="I101" t="n">
+        <v>0</v>
+      </c>
+      <c r="J101" t="n">
+        <v>0</v>
+      </c>
+      <c r="K101" t="n">
+        <v>0</v>
+      </c>
+      <c r="L101" t="n">
+        <v>1</v>
+      </c>
+      <c r="M101" t="n">
+        <v>0</v>
+      </c>
+      <c r="N101" t="n">
+        <v>0</v>
+      </c>
+      <c r="O101" t="n">
+        <v>0</v>
+      </c>
+      <c r="P101" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q101" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>0</v>
+      </c>
+      <c r="D102" t="n">
+        <v>0</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0</v>
+      </c>
+      <c r="F102" t="n">
+        <v>0</v>
+      </c>
+      <c r="G102" t="n">
+        <v>0</v>
+      </c>
+      <c r="H102" t="n">
+        <v>0</v>
+      </c>
+      <c r="I102" t="n">
+        <v>0</v>
+      </c>
+      <c r="J102" t="n">
+        <v>0</v>
+      </c>
+      <c r="K102" t="n">
+        <v>0</v>
+      </c>
+      <c r="L102" t="n">
+        <v>0</v>
+      </c>
+      <c r="M102" t="n">
+        <v>0</v>
+      </c>
+      <c r="N102" t="n">
+        <v>0</v>
+      </c>
+      <c r="O102" t="n">
+        <v>0</v>
+      </c>
+      <c r="P102" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q102" t="n">
+        <v>0</v>
+      </c>
+      <c r="R102" t="n">
+        <v>0</v>
+      </c>
+      <c r="S102" t="n">
+        <v>0</v>
+      </c>
+      <c r="T102" t="n">
+        <v>0</v>
+      </c>
+      <c r="U102" t="n">
+        <v>0</v>
+      </c>
+      <c r="V102" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>212019111</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>1</v>
+      </c>
+      <c r="D103" t="n">
+        <v>0</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0</v>
+      </c>
+      <c r="F103" t="n">
+        <v>0</v>
+      </c>
+      <c r="G103" t="n">
+        <v>1</v>
+      </c>
+      <c r="H103" t="n">
+        <v>0</v>
+      </c>
+      <c r="I103" t="n">
+        <v>0</v>
+      </c>
+      <c r="J103" t="n">
+        <v>0</v>
+      </c>
+      <c r="K103" t="n">
+        <v>0</v>
+      </c>
+      <c r="L103" t="n">
+        <v>1</v>
+      </c>
+      <c r="M103" t="n">
+        <v>0</v>
+      </c>
+      <c r="N103" t="n">
+        <v>0</v>
+      </c>
+      <c r="O103" t="n">
+        <v>0</v>
+      </c>
+      <c r="P103" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q103" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>212019111</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>1</v>
+      </c>
+      <c r="D104" t="n">
+        <v>0</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0</v>
+      </c>
+      <c r="F104" t="n">
+        <v>0</v>
+      </c>
+      <c r="G104" t="n">
+        <v>1</v>
+      </c>
+      <c r="H104" t="n">
+        <v>0</v>
+      </c>
+      <c r="I104" t="n">
+        <v>0</v>
+      </c>
+      <c r="J104" t="n">
+        <v>0</v>
+      </c>
+      <c r="K104" t="n">
+        <v>0</v>
+      </c>
+      <c r="L104" t="n">
+        <v>1</v>
+      </c>
+      <c r="M104" t="n">
+        <v>0</v>
+      </c>
+      <c r="N104" t="n">
+        <v>0</v>
+      </c>
+      <c r="O104" t="n">
+        <v>0</v>
+      </c>
+      <c r="P104" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q104" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>9202119</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>1</v>
+      </c>
+      <c r="D105" t="n">
+        <v>1</v>
+      </c>
+      <c r="E105" t="n">
+        <v>1</v>
+      </c>
+      <c r="F105" t="n">
+        <v>1</v>
+      </c>
+      <c r="G105" t="n">
+        <v>1</v>
+      </c>
+      <c r="H105" t="n">
+        <v>1</v>
+      </c>
+      <c r="I105" t="n">
+        <v>1</v>
+      </c>
+      <c r="J105" t="n">
+        <v>1</v>
+      </c>
+      <c r="K105" t="n">
+        <v>1</v>
+      </c>
+      <c r="L105" t="n">
+        <v>1</v>
+      </c>
+      <c r="M105" t="n">
+        <v>1</v>
+      </c>
+      <c r="N105" t="n">
+        <v>1</v>
+      </c>
+      <c r="O105" t="n">
+        <v>1</v>
+      </c>
+      <c r="P105" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q105" t="n">
+        <v>1</v>
+      </c>
+      <c r="R105" t="n">
+        <v>1</v>
+      </c>
+      <c r="S105" t="n">
+        <v>1</v>
+      </c>
+      <c r="T105" t="n">
+        <v>1</v>
+      </c>
+      <c r="U105" t="n">
+        <v>1</v>
+      </c>
+      <c r="V105" t="n">
+        <v>1</v>
+      </c>
+      <c r="W105" t="n">
+        <v>1</v>
+      </c>
+      <c r="X105" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y105" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z105" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA105" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB105" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC105" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD105" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF105" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>212019111</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>1</v>
+      </c>
+      <c r="D106" t="n">
+        <v>0</v>
+      </c>
+      <c r="E106" t="n">
+        <v>0</v>
+      </c>
+      <c r="F106" t="n">
+        <v>0</v>
+      </c>
+      <c r="G106" t="n">
+        <v>1</v>
+      </c>
+      <c r="H106" t="n">
+        <v>0</v>
+      </c>
+      <c r="I106" t="n">
+        <v>0</v>
+      </c>
+      <c r="J106" t="n">
+        <v>0</v>
+      </c>
+      <c r="K106" t="n">
+        <v>0</v>
+      </c>
+      <c r="L106" t="n">
+        <v>1</v>
+      </c>
+      <c r="M106" t="n">
+        <v>0</v>
+      </c>
+      <c r="N106" t="n">
+        <v>0</v>
+      </c>
+      <c r="O106" t="n">
+        <v>0</v>
+      </c>
+      <c r="P106" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q106" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>212019111</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>1</v>
+      </c>
+      <c r="D107" t="n">
+        <v>0</v>
+      </c>
+      <c r="E107" t="n">
+        <v>0</v>
+      </c>
+      <c r="F107" t="n">
+        <v>0</v>
+      </c>
+      <c r="G107" t="n">
+        <v>1</v>
+      </c>
+      <c r="H107" t="n">
+        <v>0</v>
+      </c>
+      <c r="I107" t="n">
+        <v>0</v>
+      </c>
+      <c r="J107" t="n">
+        <v>0</v>
+      </c>
+      <c r="K107" t="n">
+        <v>0</v>
+      </c>
+      <c r="L107" t="n">
+        <v>1</v>
+      </c>
+      <c r="M107" t="n">
+        <v>0</v>
+      </c>
+      <c r="N107" t="n">
+        <v>0</v>
+      </c>
+      <c r="O107" t="n">
+        <v>0</v>
+      </c>
+      <c r="P107" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q107" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>212019111</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>1</v>
+      </c>
+      <c r="D108" t="n">
+        <v>0</v>
+      </c>
+      <c r="E108" t="n">
+        <v>0</v>
+      </c>
+      <c r="F108" t="n">
+        <v>0</v>
+      </c>
+      <c r="G108" t="n">
+        <v>1</v>
+      </c>
+      <c r="H108" t="n">
+        <v>0</v>
+      </c>
+      <c r="I108" t="n">
+        <v>0</v>
+      </c>
+      <c r="J108" t="n">
+        <v>0</v>
+      </c>
+      <c r="K108" t="n">
+        <v>0</v>
+      </c>
+      <c r="L108" t="n">
+        <v>1</v>
+      </c>
+      <c r="M108" t="n">
+        <v>0</v>
+      </c>
+      <c r="N108" t="n">
+        <v>0</v>
+      </c>
+      <c r="O108" t="n">
+        <v>0</v>
+      </c>
+      <c r="P108" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q108" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>9202119</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>1</v>
+      </c>
+      <c r="D109" t="n">
+        <v>1</v>
+      </c>
+      <c r="E109" t="n">
+        <v>1</v>
+      </c>
+      <c r="F109" t="n">
+        <v>1</v>
+      </c>
+      <c r="G109" t="n">
+        <v>1</v>
+      </c>
+      <c r="H109" t="n">
+        <v>1</v>
+      </c>
+      <c r="I109" t="n">
+        <v>1</v>
+      </c>
+      <c r="J109" t="n">
+        <v>1</v>
+      </c>
+      <c r="K109" t="n">
+        <v>1</v>
+      </c>
+      <c r="L109" t="n">
+        <v>1</v>
+      </c>
+      <c r="M109" t="n">
+        <v>1</v>
+      </c>
+      <c r="N109" t="n">
+        <v>1</v>
+      </c>
+      <c r="O109" t="n">
+        <v>1</v>
+      </c>
+      <c r="P109" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q109" t="n">
+        <v>1</v>
+      </c>
+      <c r="R109" t="n">
+        <v>1</v>
+      </c>
+      <c r="S109" t="n">
+        <v>1</v>
+      </c>
+      <c r="T109" t="n">
+        <v>1</v>
+      </c>
+      <c r="U109" t="n">
+        <v>1</v>
+      </c>
+      <c r="V109" t="n">
+        <v>1</v>
+      </c>
+      <c r="W109" t="n">
+        <v>1</v>
+      </c>
+      <c r="X109" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y109" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z109" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA109" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB109" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC109" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD109" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE109" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF109" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>212019111</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>1</v>
+      </c>
+      <c r="D110" t="n">
+        <v>0</v>
+      </c>
+      <c r="E110" t="n">
+        <v>0</v>
+      </c>
+      <c r="F110" t="n">
+        <v>0</v>
+      </c>
+      <c r="G110" t="n">
+        <v>1</v>
+      </c>
+      <c r="H110" t="n">
+        <v>0</v>
+      </c>
+      <c r="I110" t="n">
+        <v>0</v>
+      </c>
+      <c r="J110" t="n">
+        <v>0</v>
+      </c>
+      <c r="K110" t="n">
+        <v>0</v>
+      </c>
+      <c r="L110" t="n">
+        <v>1</v>
+      </c>
+      <c r="M110" t="n">
+        <v>0</v>
+      </c>
+      <c r="N110" t="n">
+        <v>0</v>
+      </c>
+      <c r="O110" t="n">
+        <v>0</v>
+      </c>
+      <c r="P110" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q110" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>9202119</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Anhmedsabr</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>1</v>
+      </c>
+      <c r="D111" t="n">
+        <v>1</v>
+      </c>
+      <c r="E111" t="n">
+        <v>1</v>
+      </c>
+      <c r="F111" t="n">
+        <v>1</v>
+      </c>
+      <c r="G111" t="n">
+        <v>1</v>
+      </c>
+      <c r="H111" t="n">
+        <v>1</v>
+      </c>
+      <c r="I111" t="n">
+        <v>1</v>
+      </c>
+      <c r="J111" t="n">
+        <v>1</v>
+      </c>
+      <c r="K111" t="n">
+        <v>1</v>
+      </c>
+      <c r="L111" t="n">
+        <v>1</v>
+      </c>
+      <c r="M111" t="n">
+        <v>1</v>
+      </c>
+      <c r="N111" t="n">
+        <v>1</v>
+      </c>
+      <c r="O111" t="n">
+        <v>1</v>
+      </c>
+      <c r="P111" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q111" t="n">
+        <v>1</v>
+      </c>
+      <c r="R111" t="n">
+        <v>1</v>
+      </c>
+      <c r="S111" t="n">
+        <v>1</v>
+      </c>
+      <c r="T111" t="n">
+        <v>1</v>
+      </c>
+      <c r="U111" t="n">
+        <v>1</v>
+      </c>
+      <c r="V111" t="n">
+        <v>1</v>
+      </c>
+      <c r="W111" t="n">
+        <v>1</v>
+      </c>
+      <c r="X111" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y111" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z111" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA111" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB111" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC111" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD111" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE111" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF111" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>9202119</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>1</v>
+      </c>
+      <c r="D112" t="n">
+        <v>1</v>
+      </c>
+      <c r="E112" t="n">
+        <v>1</v>
+      </c>
+      <c r="F112" t="n">
+        <v>1</v>
+      </c>
+      <c r="G112" t="n">
+        <v>1</v>
+      </c>
+      <c r="H112" t="n">
+        <v>1</v>
+      </c>
+      <c r="I112" t="n">
+        <v>1</v>
+      </c>
+      <c r="J112" t="n">
+        <v>1</v>
+      </c>
+      <c r="K112" t="n">
+        <v>1</v>
+      </c>
+      <c r="L112" t="n">
+        <v>1</v>
+      </c>
+      <c r="M112" t="n">
+        <v>1</v>
+      </c>
+      <c r="N112" t="n">
+        <v>1</v>
+      </c>
+      <c r="O112" t="n">
+        <v>1</v>
+      </c>
+      <c r="P112" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q112" t="n">
+        <v>1</v>
+      </c>
+      <c r="R112" t="n">
+        <v>1</v>
+      </c>
+      <c r="S112" t="n">
+        <v>1</v>
+      </c>
+      <c r="T112" t="n">
+        <v>1</v>
+      </c>
+      <c r="U112" t="n">
+        <v>1</v>
+      </c>
+      <c r="V112" t="n">
+        <v>1</v>
+      </c>
+      <c r="W112" t="n">
+        <v>1</v>
+      </c>
+      <c r="X112" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y112" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z112" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA112" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB112" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC112" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD112" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE112" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF112" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>9202119</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Ahmedsabry</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>1</v>
+      </c>
+      <c r="D113" t="n">
+        <v>1</v>
+      </c>
+      <c r="E113" t="n">
+        <v>1</v>
+      </c>
+      <c r="F113" t="n">
+        <v>1</v>
+      </c>
+      <c r="G113" t="n">
+        <v>1</v>
+      </c>
+      <c r="H113" t="n">
+        <v>1</v>
+      </c>
+      <c r="I113" t="n">
+        <v>1</v>
+      </c>
+      <c r="J113" t="n">
+        <v>1</v>
+      </c>
+      <c r="K113" t="n">
+        <v>1</v>
+      </c>
+      <c r="L113" t="n">
+        <v>1</v>
+      </c>
+      <c r="M113" t="n">
+        <v>1</v>
+      </c>
+      <c r="N113" t="n">
+        <v>1</v>
+      </c>
+      <c r="O113" t="n">
+        <v>1</v>
+      </c>
+      <c r="P113" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q113" t="n">
+        <v>1</v>
+      </c>
+      <c r="R113" t="n">
+        <v>1</v>
+      </c>
+      <c r="S113" t="n">
+        <v>1</v>
+      </c>
+      <c r="T113" t="n">
+        <v>1</v>
+      </c>
+      <c r="U113" t="n">
+        <v>1</v>
+      </c>
+      <c r="V113" t="n">
+        <v>1</v>
+      </c>
+      <c r="W113" t="n">
+        <v>1</v>
+      </c>
+      <c r="X113" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y113" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z113" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA113" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB113" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC113" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD113" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE113" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF113" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="C114" t="n">
+        <v>0</v>
+      </c>
+      <c r="D114" t="n">
+        <v>0</v>
+      </c>
+      <c r="E114" t="n">
+        <v>0</v>
+      </c>
+      <c r="F114" t="n">
+        <v>0</v>
+      </c>
+      <c r="G114" t="n">
+        <v>0</v>
+      </c>
+      <c r="H114" t="n">
+        <v>0</v>
+      </c>
+      <c r="I114" t="n">
+        <v>0</v>
+      </c>
+      <c r="J114" t="n">
+        <v>1</v>
+      </c>
+      <c r="K114" t="n">
+        <v>0</v>
+      </c>
+      <c r="L114" t="n">
+        <v>0</v>
+      </c>
+      <c r="M114" t="n">
+        <v>0</v>
+      </c>
+      <c r="N114" t="n">
+        <v>0</v>
+      </c>
+      <c r="O114" t="n">
+        <v>0</v>
+      </c>
+      <c r="P114" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q114" t="n">
+        <v>0</v>
+      </c>
+      <c r="R114" t="n">
+        <v>0</v>
+      </c>
+      <c r="S114" t="n">
+        <v>1</v>
+      </c>
+      <c r="T114" t="n">
+        <v>0</v>
+      </c>
+      <c r="U114" t="n">
+        <v>0</v>
+      </c>
+      <c r="V114" t="n">
+        <v>0</v>
+      </c>
+      <c r="W114" t="n">
+        <v>0</v>
+      </c>
+      <c r="X114" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y114" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z114" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA114" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB114" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="C115" t="n">
+        <v>0</v>
+      </c>
+      <c r="D115" t="n">
+        <v>0</v>
+      </c>
+      <c r="E115" t="n">
+        <v>0</v>
+      </c>
+      <c r="F115" t="n">
+        <v>0</v>
+      </c>
+      <c r="G115" t="n">
+        <v>0</v>
+      </c>
+      <c r="H115" t="n">
+        <v>0</v>
+      </c>
+      <c r="I115" t="n">
+        <v>0</v>
+      </c>
+      <c r="J115" t="n">
+        <v>0</v>
+      </c>
+      <c r="K115" t="n">
+        <v>1</v>
+      </c>
+      <c r="L115" t="n">
+        <v>1</v>
+      </c>
+      <c r="M115" t="n">
+        <v>0</v>
+      </c>
+      <c r="N115" t="n">
+        <v>0</v>
+      </c>
+      <c r="O115" t="n">
+        <v>0</v>
+      </c>
+      <c r="P115" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q115" t="n">
+        <v>0</v>
+      </c>
+      <c r="R115" t="n">
+        <v>0</v>
+      </c>
+      <c r="S115" t="n">
+        <v>1</v>
+      </c>
+      <c r="T115" t="n">
+        <v>1</v>
+      </c>
+      <c r="U115" t="n">
+        <v>0</v>
+      </c>
+      <c r="V115" t="n">
+        <v>0</v>
+      </c>
+      <c r="W115" t="n">
+        <v>0</v>
+      </c>
+      <c r="X115" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y115" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z115" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA115" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB115" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC115" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD115" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE115" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF115" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="C116" t="n">
+        <v>1</v>
+      </c>
+      <c r="D116" t="n">
+        <v>0</v>
+      </c>
+      <c r="E116" t="n">
+        <v>0</v>
+      </c>
+      <c r="F116" t="n">
+        <v>0</v>
+      </c>
+      <c r="G116" t="n">
+        <v>1</v>
+      </c>
+      <c r="H116" t="n">
+        <v>0</v>
+      </c>
+      <c r="I116" t="n">
+        <v>0</v>
+      </c>
+      <c r="J116" t="n">
+        <v>1</v>
+      </c>
+      <c r="K116" t="n">
+        <v>0</v>
+      </c>
+      <c r="L116" t="n">
+        <v>0</v>
+      </c>
+      <c r="M116" t="n">
+        <v>1</v>
+      </c>
+      <c r="N116" t="n">
+        <v>0</v>
+      </c>
+      <c r="O116" t="n">
+        <v>1</v>
+      </c>
+      <c r="P116" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q116" t="n">
+        <v>1</v>
+      </c>
+      <c r="R116" t="n">
+        <v>0</v>
+      </c>
+      <c r="S116" t="n">
+        <v>1</v>
+      </c>
+      <c r="T116" t="n">
+        <v>0</v>
+      </c>
+      <c r="U116" t="n">
+        <v>0</v>
+      </c>
+      <c r="V116" t="n">
+        <v>1</v>
+      </c>
+      <c r="W116" t="n">
+        <v>0</v>
+      </c>
+      <c r="X116" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y116" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA116" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD116" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF116" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="C117" t="n">
+        <v>0</v>
+      </c>
+      <c r="D117" t="n">
+        <v>0</v>
+      </c>
+      <c r="E117" t="n">
+        <v>0</v>
+      </c>
+      <c r="F117" t="n">
+        <v>0</v>
+      </c>
+      <c r="G117" t="n">
+        <v>0</v>
+      </c>
+      <c r="H117" t="n">
+        <v>0</v>
+      </c>
+      <c r="I117" t="n">
+        <v>0</v>
+      </c>
+      <c r="J117" t="n">
+        <v>0</v>
+      </c>
+      <c r="K117" t="n">
+        <v>0</v>
+      </c>
+      <c r="L117" t="n">
+        <v>0</v>
+      </c>
+      <c r="M117" t="n">
+        <v>0</v>
+      </c>
+      <c r="N117" t="n">
+        <v>0</v>
+      </c>
+      <c r="O117" t="n">
+        <v>0</v>
+      </c>
+      <c r="P117" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q117" t="n">
+        <v>0</v>
+      </c>
+      <c r="R117" t="n">
+        <v>0</v>
+      </c>
+      <c r="S117" t="n">
+        <v>0</v>
+      </c>
+      <c r="T117" t="n">
+        <v>0</v>
+      </c>
+      <c r="U117" t="n">
+        <v>0</v>
+      </c>
+      <c r="V117" t="n">
+        <v>0</v>
+      </c>
+      <c r="W117" t="n">
+        <v>0</v>
+      </c>
+      <c r="X117" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y117" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z117" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA117" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB117" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="C118" t="n">
+        <v>0</v>
+      </c>
+      <c r="D118" t="n">
+        <v>0</v>
+      </c>
+      <c r="E118" t="n">
+        <v>0</v>
+      </c>
+      <c r="F118" t="n">
+        <v>0</v>
+      </c>
+      <c r="G118" t="n">
+        <v>0</v>
+      </c>
+      <c r="H118" t="n">
+        <v>0</v>
+      </c>
+      <c r="I118" t="n">
+        <v>0</v>
+      </c>
+      <c r="J118" t="n">
+        <v>1</v>
+      </c>
+      <c r="K118" t="n">
+        <v>0</v>
+      </c>
+      <c r="L118" t="n">
+        <v>0</v>
+      </c>
+      <c r="M118" t="n">
+        <v>0</v>
+      </c>
+      <c r="N118" t="n">
+        <v>0</v>
+      </c>
+      <c r="O118" t="n">
+        <v>0</v>
+      </c>
+      <c r="P118" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q118" t="n">
+        <v>0</v>
+      </c>
+      <c r="R118" t="n">
+        <v>0</v>
+      </c>
+      <c r="S118" t="n">
+        <v>1</v>
+      </c>
+      <c r="T118" t="n">
+        <v>0</v>
+      </c>
+      <c r="U118" t="n">
+        <v>0</v>
+      </c>
+      <c r="V118" t="n">
+        <v>0</v>
+      </c>
+      <c r="W118" t="n">
+        <v>0</v>
+      </c>
+      <c r="X118" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y118" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z118" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA118" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB118" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="C119" t="n">
+        <v>0</v>
+      </c>
+      <c r="D119" t="n">
+        <v>0</v>
+      </c>
+      <c r="E119" t="n">
+        <v>0</v>
+      </c>
+      <c r="F119" t="n">
+        <v>0</v>
+      </c>
+      <c r="G119" t="n">
+        <v>0</v>
+      </c>
+      <c r="H119" t="n">
+        <v>0</v>
+      </c>
+      <c r="I119" t="n">
+        <v>0</v>
+      </c>
+      <c r="J119" t="n">
+        <v>0</v>
+      </c>
+      <c r="K119" t="n">
+        <v>0</v>
+      </c>
+      <c r="L119" t="n">
+        <v>0</v>
+      </c>
+      <c r="M119" t="n">
+        <v>0</v>
+      </c>
+      <c r="N119" t="n">
+        <v>0</v>
+      </c>
+      <c r="O119" t="n">
+        <v>0</v>
+      </c>
+      <c r="P119" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q119" t="n">
+        <v>0</v>
+      </c>
+      <c r="R119" t="n">
+        <v>0</v>
+      </c>
+      <c r="S119" t="n">
+        <v>0</v>
+      </c>
+      <c r="T119" t="n">
+        <v>0</v>
+      </c>
+      <c r="U119" t="n">
+        <v>0</v>
+      </c>
+      <c r="V119" t="n">
+        <v>0</v>
+      </c>
+      <c r="W119" t="n">
+        <v>0</v>
+      </c>
+      <c r="X119" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y119" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z119" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA119" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB119" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="C120" t="n">
+        <v>0</v>
+      </c>
+      <c r="D120" t="n">
+        <v>0</v>
+      </c>
+      <c r="E120" t="n">
+        <v>0</v>
+      </c>
+      <c r="F120" t="n">
+        <v>0</v>
+      </c>
+      <c r="G120" t="n">
+        <v>0</v>
+      </c>
+      <c r="H120" t="n">
+        <v>0</v>
+      </c>
+      <c r="I120" t="n">
+        <v>0</v>
+      </c>
+      <c r="J120" t="n">
+        <v>0</v>
+      </c>
+      <c r="K120" t="n">
+        <v>0</v>
+      </c>
+      <c r="L120" t="n">
+        <v>0</v>
+      </c>
+      <c r="M120" t="n">
+        <v>0</v>
+      </c>
+      <c r="N120" t="n">
+        <v>0</v>
+      </c>
+      <c r="O120" t="n">
+        <v>0</v>
+      </c>
+      <c r="P120" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q120" t="n">
+        <v>0</v>
+      </c>
+      <c r="R120" t="n">
+        <v>0</v>
+      </c>
+      <c r="S120" t="n">
+        <v>0</v>
+      </c>
+      <c r="T120" t="n">
+        <v>0</v>
+      </c>
+      <c r="U120" t="n">
+        <v>0</v>
+      </c>
+      <c r="V120" t="n">
+        <v>0</v>
+      </c>
+      <c r="W120" t="n">
+        <v>0</v>
+      </c>
+      <c r="X120" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y120" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF120" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="C121" t="n">
+        <v>0</v>
+      </c>
+      <c r="D121" t="n">
+        <v>0</v>
+      </c>
+      <c r="E121" t="n">
+        <v>0</v>
+      </c>
+      <c r="F121" t="n">
+        <v>0</v>
+      </c>
+      <c r="G121" t="n">
+        <v>0</v>
+      </c>
+      <c r="H121" t="n">
+        <v>0</v>
+      </c>
+      <c r="I121" t="n">
+        <v>0</v>
+      </c>
+      <c r="J121" t="n">
+        <v>0</v>
+      </c>
+      <c r="K121" t="n">
+        <v>1</v>
+      </c>
+      <c r="L121" t="n">
+        <v>1</v>
+      </c>
+      <c r="M121" t="n">
+        <v>0</v>
+      </c>
+      <c r="N121" t="n">
+        <v>0</v>
+      </c>
+      <c r="O121" t="n">
+        <v>0</v>
+      </c>
+      <c r="P121" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q121" t="n">
+        <v>0</v>
+      </c>
+      <c r="R121" t="n">
+        <v>0</v>
+      </c>
+      <c r="S121" t="n">
+        <v>1</v>
+      </c>
+      <c r="T121" t="n">
+        <v>1</v>
+      </c>
+      <c r="U121" t="n">
+        <v>0</v>
+      </c>
+      <c r="V121" t="n">
+        <v>0</v>
+      </c>
+      <c r="W121" t="n">
+        <v>0</v>
+      </c>
+      <c r="X121" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y121" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z121" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC121" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF121" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="C122" t="n">
+        <v>0</v>
+      </c>
+      <c r="D122" t="n">
+        <v>0</v>
+      </c>
+      <c r="E122" t="n">
+        <v>0</v>
+      </c>
+      <c r="F122" t="n">
+        <v>0</v>
+      </c>
+      <c r="G122" t="n">
+        <v>0</v>
+      </c>
+      <c r="H122" t="n">
+        <v>0</v>
+      </c>
+      <c r="I122" t="n">
+        <v>0</v>
+      </c>
+      <c r="J122" t="n">
+        <v>0</v>
+      </c>
+      <c r="K122" t="n">
+        <v>0</v>
+      </c>
+      <c r="L122" t="n">
+        <v>0</v>
+      </c>
+      <c r="M122" t="n">
+        <v>0</v>
+      </c>
+      <c r="N122" t="n">
+        <v>0</v>
+      </c>
+      <c r="O122" t="n">
+        <v>0</v>
+      </c>
+      <c r="P122" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q122" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="C123" t="n">
+        <v>0</v>
+      </c>
+      <c r="D123" t="n">
+        <v>0</v>
+      </c>
+      <c r="E123" t="n">
+        <v>0</v>
+      </c>
+      <c r="F123" t="n">
+        <v>0</v>
+      </c>
+      <c r="G123" t="n">
+        <v>1</v>
+      </c>
+      <c r="H123" t="n">
+        <v>0</v>
+      </c>
+      <c r="I123" t="n">
+        <v>0</v>
+      </c>
+      <c r="J123" t="n">
+        <v>0</v>
+      </c>
+      <c r="K123" t="n">
+        <v>1</v>
+      </c>
+      <c r="L123" t="n">
+        <v>0</v>
+      </c>
+      <c r="M123" t="n">
+        <v>0</v>
+      </c>
+      <c r="N123" t="n">
+        <v>0</v>
+      </c>
+      <c r="O123" t="n">
+        <v>0</v>
+      </c>
+      <c r="P123" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q123" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>9202119</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>AhmedSabry~</t>
+        </is>
+      </c>
+      <c r="C124" t="n">
+        <v>1</v>
+      </c>
+      <c r="D124" t="n">
+        <v>1</v>
+      </c>
+      <c r="E124" t="n">
+        <v>1</v>
+      </c>
+      <c r="F124" t="n">
+        <v>1</v>
+      </c>
+      <c r="G124" t="n">
+        <v>1</v>
+      </c>
+      <c r="H124" t="n">
+        <v>1</v>
+      </c>
+      <c r="I124" t="n">
+        <v>1</v>
+      </c>
+      <c r="J124" t="n">
+        <v>1</v>
+      </c>
+      <c r="K124" t="n">
+        <v>1</v>
+      </c>
+      <c r="L124" t="n">
+        <v>1</v>
+      </c>
+      <c r="M124" t="n">
+        <v>1</v>
+      </c>
+      <c r="N124" t="n">
+        <v>1</v>
+      </c>
+      <c r="O124" t="n">
+        <v>1</v>
+      </c>
+      <c r="P124" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q124" t="n">
+        <v>1</v>
+      </c>
+      <c r="R124" t="n">
+        <v>1</v>
+      </c>
+      <c r="S124" t="n">
+        <v>1</v>
+      </c>
+      <c r="T124" t="n">
+        <v>1</v>
+      </c>
+      <c r="U124" t="n">
+        <v>1</v>
+      </c>
+      <c r="V124" t="n">
+        <v>1</v>
+      </c>
+      <c r="W124" t="n">
+        <v>1</v>
+      </c>
+      <c r="X124" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y124" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z124" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA124" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB124" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC124" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD124" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE124" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF124" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="C125" t="n">
+        <v>0</v>
+      </c>
+      <c r="D125" t="n">
+        <v>0</v>
+      </c>
+      <c r="E125" t="n">
+        <v>0</v>
+      </c>
+      <c r="F125" t="n">
+        <v>0</v>
+      </c>
+      <c r="G125" t="n">
+        <v>0</v>
+      </c>
+      <c r="H125" t="n">
+        <v>0</v>
+      </c>
+      <c r="I125" t="n">
+        <v>0</v>
+      </c>
+      <c r="J125" t="n">
+        <v>0</v>
+      </c>
+      <c r="K125" t="n">
+        <v>0</v>
+      </c>
+      <c r="L125" t="n">
+        <v>0</v>
+      </c>
+      <c r="M125" t="n">
+        <v>0</v>
+      </c>
+      <c r="N125" t="n">
+        <v>0</v>
+      </c>
+      <c r="O125" t="n">
+        <v>0</v>
+      </c>
+      <c r="P125" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q125" t="n">
+        <v>0</v>
+      </c>
+      <c r="R125" t="n">
+        <v>0</v>
+      </c>
+      <c r="S125" t="n">
+        <v>0</v>
+      </c>
+      <c r="T125" t="n">
+        <v>0</v>
+      </c>
+      <c r="U125" t="n">
+        <v>0</v>
+      </c>
+      <c r="V125" t="n">
+        <v>0</v>
+      </c>
+      <c r="W125" t="n">
+        <v>0</v>
+      </c>
+      <c r="X125" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y125" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z125" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA125" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB125" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC125" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD125" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE125" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF125" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="C126" t="n">
+        <v>1</v>
+      </c>
+      <c r="D126" t="n">
+        <v>0</v>
+      </c>
+      <c r="E126" t="n">
+        <v>0</v>
+      </c>
+      <c r="F126" t="n">
+        <v>0</v>
+      </c>
+      <c r="G126" t="n">
+        <v>1</v>
+      </c>
+      <c r="H126" t="n">
+        <v>0</v>
+      </c>
+      <c r="I126" t="n">
+        <v>0</v>
+      </c>
+      <c r="J126" t="n">
+        <v>1</v>
+      </c>
+      <c r="K126" t="n">
+        <v>0</v>
+      </c>
+      <c r="L126" t="n">
+        <v>0</v>
+      </c>
+      <c r="M126" t="n">
+        <v>1</v>
+      </c>
+      <c r="N126" t="n">
+        <v>0</v>
+      </c>
+      <c r="O126" t="n">
+        <v>1</v>
+      </c>
+      <c r="P126" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q126" t="n">
+        <v>1</v>
+      </c>
+      <c r="R126" t="n">
+        <v>0</v>
+      </c>
+      <c r="S126" t="n">
+        <v>1</v>
+      </c>
+      <c r="T126" t="n">
+        <v>0</v>
+      </c>
+      <c r="U126" t="n">
+        <v>0</v>
+      </c>
+      <c r="V126" t="n">
+        <v>1</v>
+      </c>
+      <c r="W126" t="n">
+        <v>0</v>
+      </c>
+      <c r="X126" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y126" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z126" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA126" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB126" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC126" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD126" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE126" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF126" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="C127" t="n">
+        <v>1</v>
+      </c>
+      <c r="D127" t="n">
+        <v>0</v>
+      </c>
+      <c r="E127" t="n">
+        <v>0</v>
+      </c>
+      <c r="F127" t="n">
+        <v>0</v>
+      </c>
+      <c r="G127" t="n">
+        <v>1</v>
+      </c>
+      <c r="H127" t="n">
+        <v>0</v>
+      </c>
+      <c r="I127" t="n">
+        <v>0</v>
+      </c>
+      <c r="J127" t="n">
+        <v>1</v>
+      </c>
+      <c r="K127" t="n">
+        <v>0</v>
+      </c>
+      <c r="L127" t="n">
+        <v>0</v>
+      </c>
+      <c r="M127" t="n">
+        <v>1</v>
+      </c>
+      <c r="N127" t="n">
+        <v>0</v>
+      </c>
+      <c r="O127" t="n">
+        <v>1</v>
+      </c>
+      <c r="P127" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q127" t="n">
+        <v>1</v>
+      </c>
+      <c r="R127" t="n">
+        <v>0</v>
+      </c>
+      <c r="S127" t="n">
+        <v>1</v>
+      </c>
+      <c r="T127" t="n">
+        <v>0</v>
+      </c>
+      <c r="U127" t="n">
+        <v>0</v>
+      </c>
+      <c r="V127" t="n">
+        <v>1</v>
+      </c>
+      <c r="W127" t="n">
+        <v>0</v>
+      </c>
+      <c r="X127" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y127" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z127" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA127" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB127" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC127" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD127" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE127" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF127" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG127" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH127" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI127" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ127" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK127" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL127" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM127" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN127" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO127" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP127" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ127" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR127" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS127" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT127" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU127" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="C128" t="n">
+        <v>0</v>
+      </c>
+      <c r="D128" t="n">
+        <v>0</v>
+      </c>
+      <c r="E128" t="n">
+        <v>0</v>
+      </c>
+      <c r="F128" t="n">
+        <v>0</v>
+      </c>
+      <c r="G128" t="n">
+        <v>0</v>
+      </c>
+      <c r="H128" t="n">
+        <v>0</v>
+      </c>
+      <c r="I128" t="n">
+        <v>0</v>
+      </c>
+      <c r="J128" t="n">
+        <v>0</v>
+      </c>
+      <c r="K128" t="n">
+        <v>0</v>
+      </c>
+      <c r="L128" t="n">
+        <v>0</v>
+      </c>
+      <c r="M128" t="n">
+        <v>0</v>
+      </c>
+      <c r="N128" t="n">
+        <v>0</v>
+      </c>
+      <c r="O128" t="n">
+        <v>0</v>
+      </c>
+      <c r="P128" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q128" t="n">
+        <v>0</v>
+      </c>
+      <c r="R128" t="n">
+        <v>0</v>
+      </c>
+      <c r="S128" t="n">
+        <v>0</v>
+      </c>
+      <c r="T128" t="n">
+        <v>0</v>
+      </c>
+      <c r="U128" t="n">
+        <v>0</v>
+      </c>
+      <c r="V128" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="C129" t="n">
+        <v>0</v>
+      </c>
+      <c r="D129" t="n">
+        <v>0</v>
+      </c>
+      <c r="E129" t="n">
+        <v>0</v>
+      </c>
+      <c r="F129" t="n">
+        <v>0</v>
+      </c>
+      <c r="G129" t="n">
+        <v>0</v>
+      </c>
+      <c r="H129" t="n">
+        <v>0</v>
+      </c>
+      <c r="I129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J129" t="n">
+        <v>0</v>
+      </c>
+      <c r="K129" t="n">
+        <v>0</v>
+      </c>
+      <c r="L129" t="n">
+        <v>0</v>
+      </c>
+      <c r="M129" t="n">
+        <v>0</v>
+      </c>
+      <c r="N129" t="n">
+        <v>0</v>
+      </c>
+      <c r="O129" t="n">
+        <v>0</v>
+      </c>
+      <c r="P129" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q129" t="n">
+        <v>0</v>
+      </c>
+      <c r="R129" t="n">
+        <v>0</v>
+      </c>
+      <c r="S129" t="n">
+        <v>0</v>
+      </c>
+      <c r="T129" t="n">
+        <v>0</v>
+      </c>
+      <c r="U129" t="n">
+        <v>0</v>
+      </c>
+      <c r="V129" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="C130" t="n">
+        <v>0</v>
+      </c>
+      <c r="D130" t="n">
+        <v>0</v>
+      </c>
+      <c r="E130" t="n">
+        <v>0</v>
+      </c>
+      <c r="F130" t="n">
+        <v>0</v>
+      </c>
+      <c r="G130" t="n">
+        <v>0</v>
+      </c>
+      <c r="H130" t="n">
+        <v>0</v>
+      </c>
+      <c r="I130" t="n">
+        <v>0</v>
+      </c>
+      <c r="J130" t="n">
+        <v>0</v>
+      </c>
+      <c r="K130" t="n">
+        <v>0</v>
+      </c>
+      <c r="L130" t="n">
+        <v>0</v>
+      </c>
+      <c r="M130" t="n">
+        <v>0</v>
+      </c>
+      <c r="N130" t="n">
+        <v>0</v>
+      </c>
+      <c r="O130" t="n">
+        <v>0</v>
+      </c>
+      <c r="P130" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q130" t="n">
+        <v>0</v>
+      </c>
+      <c r="R130" t="n">
+        <v>0</v>
+      </c>
+      <c r="S130" t="n">
+        <v>0</v>
+      </c>
+      <c r="T130" t="n">
+        <v>0</v>
+      </c>
+      <c r="U130" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="C131" t="n">
+        <v>0</v>
+      </c>
+      <c r="D131" t="n">
+        <v>0</v>
+      </c>
+      <c r="E131" t="n">
+        <v>0</v>
+      </c>
+      <c r="F131" t="n">
+        <v>0</v>
+      </c>
+      <c r="G131" t="n">
+        <v>0</v>
+      </c>
+      <c r="H131" t="n">
+        <v>0</v>
+      </c>
+      <c r="I131" t="n">
+        <v>0</v>
+      </c>
+      <c r="J131" t="n">
+        <v>0</v>
+      </c>
+      <c r="K131" t="n">
+        <v>0</v>
+      </c>
+      <c r="L131" t="n">
+        <v>0</v>
+      </c>
+      <c r="M131" t="n">
+        <v>0</v>
+      </c>
+      <c r="N131" t="n">
+        <v>0</v>
+      </c>
+      <c r="O131" t="n">
+        <v>0</v>
+      </c>
+      <c r="P131" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q131" t="n">
+        <v>0</v>
+      </c>
+      <c r="R131" t="n">
+        <v>0</v>
+      </c>
+      <c r="S131" t="n">
+        <v>0</v>
+      </c>
+      <c r="T131" t="n">
+        <v>0</v>
+      </c>
+      <c r="U131" t="n">
+        <v>0</v>
+      </c>
+      <c r="V131" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr"/>
+      <c r="B132" t="inlineStr"/>
+      <c r="C132" t="n">
+        <v>0</v>
+      </c>
+      <c r="D132" t="n">
+        <v>0</v>
+      </c>
+      <c r="E132" t="n">
+        <v>0</v>
+      </c>
+      <c r="F132" t="n">
+        <v>0</v>
+      </c>
+      <c r="G132" t="n">
+        <v>0</v>
+      </c>
+      <c r="H132" t="n">
+        <v>0</v>
+      </c>
+      <c r="I132" t="n">
+        <v>0</v>
+      </c>
+      <c r="J132" t="n">
+        <v>0</v>
+      </c>
+      <c r="K132" t="n">
+        <v>0</v>
+      </c>
+      <c r="L132" t="n">
+        <v>0</v>
+      </c>
+      <c r="M132" t="n">
+        <v>0</v>
+      </c>
+      <c r="N132" t="n">
+        <v>0</v>
+      </c>
+      <c r="O132" t="n">
+        <v>0</v>
+      </c>
+      <c r="P132" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q132" t="n">
+        <v>0</v>
+      </c>
+      <c r="R132" t="n">
+        <v>0</v>
+      </c>
+      <c r="S132" t="n">
+        <v>0</v>
+      </c>
+      <c r="T132" t="n">
+        <v>0</v>
+      </c>
+      <c r="U132" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
separate code in classes
</commit_message>
<xml_diff>
--- a/BubbleSheet/answers.xlsx
+++ b/BubbleSheet/answers.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:AF66"/>
+  <dimension ref="A2:AF77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5675,7 +5675,6 @@
           <t>100</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr"/>
       <c r="C66" t="n">
         <v>0</v>
       </c>
@@ -5716,6 +5715,594 @@
         <v>0</v>
       </c>
       <c r="P66" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2303</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>0</v>
+      </c>
+      <c r="D67" t="n">
+        <v>1</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0</v>
+      </c>
+      <c r="G67" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J67" t="n">
+        <v>0</v>
+      </c>
+      <c r="K67" t="n">
+        <v>0</v>
+      </c>
+      <c r="L67" t="n">
+        <v>0</v>
+      </c>
+      <c r="M67" t="n">
+        <v>0</v>
+      </c>
+      <c r="N67" t="n">
+        <v>0</v>
+      </c>
+      <c r="O67" t="n">
+        <v>0</v>
+      </c>
+      <c r="P67" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q67" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>10301</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>MohamedAhied</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>1</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0</v>
+      </c>
+      <c r="F68" t="n">
+        <v>1</v>
+      </c>
+      <c r="G68" t="n">
+        <v>0</v>
+      </c>
+      <c r="H68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" t="n">
+        <v>0</v>
+      </c>
+      <c r="K68" t="n">
+        <v>0</v>
+      </c>
+      <c r="L68" t="n">
+        <v>0</v>
+      </c>
+      <c r="M68" t="n">
+        <v>0</v>
+      </c>
+      <c r="N68" t="n">
+        <v>0</v>
+      </c>
+      <c r="O68" t="n">
+        <v>0</v>
+      </c>
+      <c r="P68" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q68" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2303</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>0</v>
+      </c>
+      <c r="D69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0</v>
+      </c>
+      <c r="G69" t="n">
+        <v>0</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J69" t="n">
+        <v>0</v>
+      </c>
+      <c r="K69" t="n">
+        <v>0</v>
+      </c>
+      <c r="L69" t="n">
+        <v>0</v>
+      </c>
+      <c r="M69" t="n">
+        <v>0</v>
+      </c>
+      <c r="N69" t="n">
+        <v>0</v>
+      </c>
+      <c r="O69" t="n">
+        <v>0</v>
+      </c>
+      <c r="P69" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q69" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2303</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>0</v>
+      </c>
+      <c r="D70" t="n">
+        <v>1</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" t="n">
+        <v>0</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0</v>
+      </c>
+      <c r="J70" t="n">
+        <v>0</v>
+      </c>
+      <c r="K70" t="n">
+        <v>0</v>
+      </c>
+      <c r="L70" t="n">
+        <v>0</v>
+      </c>
+      <c r="M70" t="n">
+        <v>0</v>
+      </c>
+      <c r="N70" t="n">
+        <v>0</v>
+      </c>
+      <c r="O70" t="n">
+        <v>0</v>
+      </c>
+      <c r="P70" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q70" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>10301</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>MohamedAhied</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>1</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" t="n">
+        <v>1</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0</v>
+      </c>
+      <c r="J71" t="n">
+        <v>0</v>
+      </c>
+      <c r="K71" t="n">
+        <v>0</v>
+      </c>
+      <c r="L71" t="n">
+        <v>0</v>
+      </c>
+      <c r="M71" t="n">
+        <v>0</v>
+      </c>
+      <c r="N71" t="n">
+        <v>0</v>
+      </c>
+      <c r="O71" t="n">
+        <v>0</v>
+      </c>
+      <c r="P71" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q71" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>0</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0</v>
+      </c>
+      <c r="I72" t="n">
+        <v>0</v>
+      </c>
+      <c r="J72" t="n">
+        <v>0</v>
+      </c>
+      <c r="K72" t="n">
+        <v>0</v>
+      </c>
+      <c r="L72" t="n">
+        <v>0</v>
+      </c>
+      <c r="M72" t="n">
+        <v>1</v>
+      </c>
+      <c r="N72" t="n">
+        <v>0</v>
+      </c>
+      <c r="O72" t="n">
+        <v>0</v>
+      </c>
+      <c r="P72" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q72" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>09211</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>0</v>
+      </c>
+      <c r="D73" t="n">
+        <v>1</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0</v>
+      </c>
+      <c r="G73" t="n">
+        <v>1</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0</v>
+      </c>
+      <c r="I73" t="n">
+        <v>0</v>
+      </c>
+      <c r="J73" t="n">
+        <v>0</v>
+      </c>
+      <c r="K73" t="n">
+        <v>0</v>
+      </c>
+      <c r="L73" t="n">
+        <v>0</v>
+      </c>
+      <c r="M73" t="n">
+        <v>0</v>
+      </c>
+      <c r="N73" t="n">
+        <v>1</v>
+      </c>
+      <c r="O73" t="n">
+        <v>0</v>
+      </c>
+      <c r="P73" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q73" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2303</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>0</v>
+      </c>
+      <c r="D74" t="n">
+        <v>1</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0</v>
+      </c>
+      <c r="H74" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" t="n">
+        <v>0</v>
+      </c>
+      <c r="J74" t="n">
+        <v>0</v>
+      </c>
+      <c r="K74" t="n">
+        <v>0</v>
+      </c>
+      <c r="L74" t="n">
+        <v>0</v>
+      </c>
+      <c r="M74" t="n">
+        <v>0</v>
+      </c>
+      <c r="N74" t="n">
+        <v>0</v>
+      </c>
+      <c r="O74" t="n">
+        <v>0</v>
+      </c>
+      <c r="P74" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q74" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>10301</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>MohamedAhied</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>1</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0</v>
+      </c>
+      <c r="F75" t="n">
+        <v>1</v>
+      </c>
+      <c r="G75" t="n">
+        <v>0</v>
+      </c>
+      <c r="H75" t="n">
+        <v>0</v>
+      </c>
+      <c r="I75" t="n">
+        <v>0</v>
+      </c>
+      <c r="J75" t="n">
+        <v>0</v>
+      </c>
+      <c r="K75" t="n">
+        <v>0</v>
+      </c>
+      <c r="L75" t="n">
+        <v>0</v>
+      </c>
+      <c r="M75" t="n">
+        <v>0</v>
+      </c>
+      <c r="N75" t="n">
+        <v>0</v>
+      </c>
+      <c r="O75" t="n">
+        <v>0</v>
+      </c>
+      <c r="P75" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q75" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>0</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H76" t="n">
+        <v>0</v>
+      </c>
+      <c r="I76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J76" t="n">
+        <v>0</v>
+      </c>
+      <c r="K76" t="n">
+        <v>0</v>
+      </c>
+      <c r="L76" t="n">
+        <v>0</v>
+      </c>
+      <c r="M76" t="n">
+        <v>1</v>
+      </c>
+      <c r="N76" t="n">
+        <v>0</v>
+      </c>
+      <c r="O76" t="n">
+        <v>0</v>
+      </c>
+      <c r="P76" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q76" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>09211</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr"/>
+      <c r="C77" t="n">
+        <v>0</v>
+      </c>
+      <c r="D77" t="n">
+        <v>1</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0</v>
+      </c>
+      <c r="G77" t="n">
+        <v>1</v>
+      </c>
+      <c r="H77" t="n">
+        <v>0</v>
+      </c>
+      <c r="I77" t="n">
+        <v>0</v>
+      </c>
+      <c r="J77" t="n">
+        <v>0</v>
+      </c>
+      <c r="K77" t="n">
+        <v>0</v>
+      </c>
+      <c r="L77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M77" t="n">
+        <v>0</v>
+      </c>
+      <c r="N77" t="n">
+        <v>1</v>
+      </c>
+      <c r="O77" t="n">
+        <v>0</v>
+      </c>
+      <c r="P77" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q77" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Edit paths in bubble sheet
</commit_message>
<xml_diff>
--- a/BubbleSheet/answers.xlsx
+++ b/BubbleSheet/answers.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:AF138"/>
+  <dimension ref="A2:AF143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11133,7 +11133,6 @@
           <t>0082018</t>
         </is>
       </c>
-      <c r="B138" t="inlineStr"/>
       <c r="C138" t="n">
         <v>0</v>
       </c>
@@ -11222,6 +11221,497 @@
         <v>0</v>
       </c>
       <c r="AF138" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>826</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>AbnedAK</t>
+        </is>
+      </c>
+      <c r="C139" t="n">
+        <v>0</v>
+      </c>
+      <c r="D139" t="n">
+        <v>0</v>
+      </c>
+      <c r="E139" t="n">
+        <v>0</v>
+      </c>
+      <c r="F139" t="n">
+        <v>0</v>
+      </c>
+      <c r="G139" t="n">
+        <v>1</v>
+      </c>
+      <c r="H139" t="n">
+        <v>0</v>
+      </c>
+      <c r="I139" t="n">
+        <v>0</v>
+      </c>
+      <c r="J139" t="n">
+        <v>0</v>
+      </c>
+      <c r="K139" t="n">
+        <v>0</v>
+      </c>
+      <c r="L139" t="n">
+        <v>0</v>
+      </c>
+      <c r="M139" t="n">
+        <v>0</v>
+      </c>
+      <c r="N139" t="n">
+        <v>0</v>
+      </c>
+      <c r="O139" t="n">
+        <v>0</v>
+      </c>
+      <c r="P139" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q139" t="n">
+        <v>0</v>
+      </c>
+      <c r="R139" t="n">
+        <v>0</v>
+      </c>
+      <c r="S139" t="n">
+        <v>0</v>
+      </c>
+      <c r="T139" t="n">
+        <v>0</v>
+      </c>
+      <c r="U139" t="n">
+        <v>0</v>
+      </c>
+      <c r="V139" t="n">
+        <v>0</v>
+      </c>
+      <c r="W139" t="n">
+        <v>0</v>
+      </c>
+      <c r="X139" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y139" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z139" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA139" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB139" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC139" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD139" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE139" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF139" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>810</t>
+        </is>
+      </c>
+      <c r="C140" t="n">
+        <v>1</v>
+      </c>
+      <c r="D140" t="n">
+        <v>0</v>
+      </c>
+      <c r="E140" t="n">
+        <v>0</v>
+      </c>
+      <c r="F140" t="n">
+        <v>0</v>
+      </c>
+      <c r="G140" t="n">
+        <v>0</v>
+      </c>
+      <c r="H140" t="n">
+        <v>0</v>
+      </c>
+      <c r="I140" t="n">
+        <v>0</v>
+      </c>
+      <c r="J140" t="n">
+        <v>0</v>
+      </c>
+      <c r="K140" t="n">
+        <v>0</v>
+      </c>
+      <c r="L140" t="n">
+        <v>0</v>
+      </c>
+      <c r="M140" t="n">
+        <v>0</v>
+      </c>
+      <c r="N140" t="n">
+        <v>0</v>
+      </c>
+      <c r="O140" t="n">
+        <v>1</v>
+      </c>
+      <c r="P140" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q140" t="n">
+        <v>0</v>
+      </c>
+      <c r="R140" t="n">
+        <v>0</v>
+      </c>
+      <c r="S140" t="n">
+        <v>0</v>
+      </c>
+      <c r="T140" t="n">
+        <v>1</v>
+      </c>
+      <c r="U140" t="n">
+        <v>0</v>
+      </c>
+      <c r="V140" t="n">
+        <v>0</v>
+      </c>
+      <c r="W140" t="n">
+        <v>0</v>
+      </c>
+      <c r="X140" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y140" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z140" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA140" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB140" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC140" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD140" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE140" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF140" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C141" t="n">
+        <v>1</v>
+      </c>
+      <c r="D141" t="n">
+        <v>0</v>
+      </c>
+      <c r="E141" t="n">
+        <v>0</v>
+      </c>
+      <c r="F141" t="n">
+        <v>0</v>
+      </c>
+      <c r="G141" t="n">
+        <v>1</v>
+      </c>
+      <c r="H141" t="n">
+        <v>1</v>
+      </c>
+      <c r="I141" t="n">
+        <v>1</v>
+      </c>
+      <c r="J141" t="n">
+        <v>1</v>
+      </c>
+      <c r="K141" t="n">
+        <v>0</v>
+      </c>
+      <c r="L141" t="n">
+        <v>0</v>
+      </c>
+      <c r="M141" t="n">
+        <v>0</v>
+      </c>
+      <c r="N141" t="n">
+        <v>0</v>
+      </c>
+      <c r="O141" t="n">
+        <v>0</v>
+      </c>
+      <c r="P141" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q141" t="n">
+        <v>1</v>
+      </c>
+      <c r="R141" t="n">
+        <v>0</v>
+      </c>
+      <c r="S141" t="n">
+        <v>0</v>
+      </c>
+      <c r="T141" t="n">
+        <v>1</v>
+      </c>
+      <c r="U141" t="n">
+        <v>0</v>
+      </c>
+      <c r="V141" t="n">
+        <v>0</v>
+      </c>
+      <c r="W141" t="n">
+        <v>1</v>
+      </c>
+      <c r="X141" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y141" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z141" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA141" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB141" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC141" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD141" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE141" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF141" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>79370</t>
+        </is>
+      </c>
+      <c r="C142" t="n">
+        <v>1</v>
+      </c>
+      <c r="D142" t="n">
+        <v>0</v>
+      </c>
+      <c r="E142" t="n">
+        <v>0</v>
+      </c>
+      <c r="F142" t="n">
+        <v>0</v>
+      </c>
+      <c r="G142" t="n">
+        <v>0</v>
+      </c>
+      <c r="H142" t="n">
+        <v>0</v>
+      </c>
+      <c r="I142" t="n">
+        <v>0</v>
+      </c>
+      <c r="J142" t="n">
+        <v>0</v>
+      </c>
+      <c r="K142" t="n">
+        <v>0</v>
+      </c>
+      <c r="L142" t="n">
+        <v>0</v>
+      </c>
+      <c r="M142" t="n">
+        <v>0</v>
+      </c>
+      <c r="N142" t="n">
+        <v>0</v>
+      </c>
+      <c r="O142" t="n">
+        <v>1</v>
+      </c>
+      <c r="P142" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q142" t="n">
+        <v>0</v>
+      </c>
+      <c r="R142" t="n">
+        <v>0</v>
+      </c>
+      <c r="S142" t="n">
+        <v>0</v>
+      </c>
+      <c r="T142" t="n">
+        <v>1</v>
+      </c>
+      <c r="U142" t="n">
+        <v>0</v>
+      </c>
+      <c r="V142" t="n">
+        <v>0</v>
+      </c>
+      <c r="W142" t="n">
+        <v>0</v>
+      </c>
+      <c r="X142" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y142" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF142" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>0082018</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr"/>
+      <c r="C143" t="n">
+        <v>0</v>
+      </c>
+      <c r="D143" t="n">
+        <v>0</v>
+      </c>
+      <c r="E143" t="n">
+        <v>0</v>
+      </c>
+      <c r="F143" t="n">
+        <v>0</v>
+      </c>
+      <c r="G143" t="n">
+        <v>0</v>
+      </c>
+      <c r="H143" t="n">
+        <v>0</v>
+      </c>
+      <c r="I143" t="n">
+        <v>0</v>
+      </c>
+      <c r="J143" t="n">
+        <v>0</v>
+      </c>
+      <c r="K143" t="n">
+        <v>0</v>
+      </c>
+      <c r="L143" t="n">
+        <v>0</v>
+      </c>
+      <c r="M143" t="n">
+        <v>0</v>
+      </c>
+      <c r="N143" t="n">
+        <v>0</v>
+      </c>
+      <c r="O143" t="n">
+        <v>0</v>
+      </c>
+      <c r="P143" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q143" t="n">
+        <v>0</v>
+      </c>
+      <c r="R143" t="n">
+        <v>0</v>
+      </c>
+      <c r="S143" t="n">
+        <v>0</v>
+      </c>
+      <c r="T143" t="n">
+        <v>0</v>
+      </c>
+      <c r="U143" t="n">
+        <v>0</v>
+      </c>
+      <c r="V143" t="n">
+        <v>0</v>
+      </c>
+      <c r="W143" t="n">
+        <v>0</v>
+      </c>
+      <c r="X143" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y143" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z143" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA143" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB143" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC143" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD143" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE143" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF143" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove Bubble_Data from path
</commit_message>
<xml_diff>
--- a/BubbleSheet/answers.xlsx
+++ b/BubbleSheet/answers.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:AF143"/>
+  <dimension ref="A2:AF144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11623,7 +11623,6 @@
           <t>0082018</t>
         </is>
       </c>
-      <c r="B143" t="inlineStr"/>
       <c r="C143" t="n">
         <v>0</v>
       </c>
@@ -11712,6 +11711,85 @@
         <v>0</v>
       </c>
       <c r="AF143" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr"/>
+      <c r="B144" t="inlineStr"/>
+      <c r="C144" t="n">
+        <v>0</v>
+      </c>
+      <c r="D144" t="n">
+        <v>0</v>
+      </c>
+      <c r="E144" t="n">
+        <v>0</v>
+      </c>
+      <c r="F144" t="n">
+        <v>0</v>
+      </c>
+      <c r="G144" t="n">
+        <v>0</v>
+      </c>
+      <c r="H144" t="n">
+        <v>0</v>
+      </c>
+      <c r="I144" t="n">
+        <v>0</v>
+      </c>
+      <c r="J144" t="n">
+        <v>0</v>
+      </c>
+      <c r="K144" t="n">
+        <v>1</v>
+      </c>
+      <c r="L144" t="n">
+        <v>0</v>
+      </c>
+      <c r="M144" t="n">
+        <v>0</v>
+      </c>
+      <c r="N144" t="n">
+        <v>0</v>
+      </c>
+      <c r="O144" t="n">
+        <v>0</v>
+      </c>
+      <c r="P144" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q144" t="n">
+        <v>1</v>
+      </c>
+      <c r="R144" t="n">
+        <v>0</v>
+      </c>
+      <c r="S144" t="n">
+        <v>0</v>
+      </c>
+      <c r="T144" t="n">
+        <v>0</v>
+      </c>
+      <c r="U144" t="n">
+        <v>0</v>
+      </c>
+      <c r="V144" t="n">
+        <v>0</v>
+      </c>
+      <c r="W144" t="n">
+        <v>0</v>
+      </c>
+      <c r="X144" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y144" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z144" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA144" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>